<commit_message>
Worked fix game player & tournament
</commit_message>
<xml_diff>
--- a/Portal Capital Model/2013 TestBed v.02.xlsx
+++ b/Portal Capital Model/2013 TestBed v.02.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="13095" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21840" windowHeight="13095" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sagarin Ratings 2013.03.13" sheetId="3" r:id="rId1"/>
     <sheet name="2012.03.12 Sagarin Ratings" sheetId="4" r:id="rId2"/>
-    <sheet name="TeamData" sheetId="1" r:id="rId3"/>
+    <sheet name="usaTodayNames" sheetId="5" r:id="rId3"/>
+    <sheet name="TeamData" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="IQ_CH" hidden="1">110000</definedName>
@@ -36,7 +37,7 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_MONTH" hidden="1">15000</definedName>
     <definedName name="IQ_MTD" hidden="1">800000</definedName>
-    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">41171.6034953704</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">41303.8599884259</definedName>
     <definedName name="IQ_NTM" hidden="1">6000</definedName>
     <definedName name="IQ_QTD" hidden="1">750000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
@@ -44,12 +45,12 @@
     <definedName name="IQ_YTD" hidden="1">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="144525" calcMode="autoNoTable" iterate="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="398">
   <si>
     <t>Name</t>
   </si>
@@ -1162,16 +1163,104 @@
   </si>
   <si>
     <t>Nebraska-Omaha</t>
+  </si>
+  <si>
+    <t>usaTodayTeamName</t>
+  </si>
+  <si>
+    <t>roundEliminated</t>
+  </si>
+  <si>
+    <t>Long Beach St.</t>
+  </si>
+  <si>
+    <t>No.Carolina A&amp;amp;T</t>
+  </si>
+  <si>
+    <t>Ohio St</t>
+  </si>
+  <si>
+    <t>Michigan St</t>
+  </si>
+  <si>
+    <t>St. Joseph's</t>
+  </si>
+  <si>
+    <t>Prairie View A&amp;amp;M</t>
+  </si>
+  <si>
+    <t>N.C. State</t>
+  </si>
+  <si>
+    <t>Oklahoma St.</t>
+  </si>
+  <si>
+    <t>Texas-El Paso</t>
+  </si>
+  <si>
+    <t>Colorado St.</t>
+  </si>
+  <si>
+    <t>Cal Poly SLO</t>
+  </si>
+  <si>
+    <t>Louisiana State</t>
+  </si>
+  <si>
+    <t>Iowa St.</t>
+  </si>
+  <si>
+    <t>Kent St.</t>
+  </si>
+  <si>
+    <t>Sam Houston St.</t>
+  </si>
+  <si>
+    <t>Southeastern Louisiana</t>
+  </si>
+  <si>
+    <t>Weber St.</t>
+  </si>
+  <si>
+    <t>Alabama A&amp;amp;M</t>
+  </si>
+  <si>
+    <t>Morgan St.</t>
+  </si>
+  <si>
+    <t>Northwestern St.</t>
+  </si>
+  <si>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>Kansas St.</t>
+  </si>
+  <si>
+    <t>New Mexico St.</t>
+  </si>
+  <si>
+    <t>Texas-San Antonio</t>
+  </si>
+  <si>
+    <t>Florida St.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1214,19 +1303,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_Sheet3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6413,8 +6506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D346"/>
   <sheetViews>
-    <sheetView topLeftCell="A343" workbookViewId="0">
-      <selection sqref="A1:D346"/>
+    <sheetView topLeftCell="A315" workbookViewId="0">
+      <selection activeCell="D346" sqref="D346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11270,10 +11363,428 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:A80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11281,9 +11792,11 @@
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11296,8 +11809,14 @@
       <c r="D1" s="1" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11311,8 +11830,15 @@
         <f>VLOOKUP(C2,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>76.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="e">
+        <f>VLOOKUP(A2,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11326,8 +11852,15 @@
         <f>VLOOKUP(C3,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>74.84</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="e">
+        <f>VLOOKUP(A3,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -11342,8 +11875,15 @@
         <f>VLOOKUP(C4,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>80.87</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="e">
+        <f>VLOOKUP(A4,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -11358,8 +11898,15 @@
         <f>VLOOKUP(C5,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>78.11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="str">
+        <f>VLOOKUP(A5,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Montana</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -11374,8 +11921,15 @@
         <f>VLOOKUP(C6,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>82.34</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="e">
+        <f>VLOOKUP(A6,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11390,8 +11944,15 @@
         <f>VLOOKUP(C7,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.61</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="e">
+        <f>VLOOKUP(A7,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -11406,8 +11967,15 @@
         <f>VLOOKUP(C8,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83.69</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="e">
+        <f>VLOOKUP(A8,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -11422,8 +11990,15 @@
         <f>VLOOKUP(C9,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>80.44</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="str">
+        <f>VLOOKUP(A9,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Southern Miss</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -11438,8 +12013,14 @@
         <f>VLOOKUP(C10,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>86.08</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -11454,8 +12035,15 @@
         <f>VLOOKUP(C11,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>84.48</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="e">
+        <f>VLOOKUP(A11,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -11470,8 +12058,15 @@
         <f>VLOOKUP(C12,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83.69</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="e">
+        <f>VLOOKUP(A12,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -11486,8 +12081,15 @@
         <f>VLOOKUP(C13,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>86.45</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="str">
+        <f>VLOOKUP(A13,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Vanderbilt</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -11502,8 +12104,15 @@
         <f>VLOOKUP(C14,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>90.86</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="str">
+        <f>VLOOKUP(A14,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Wisconsin</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -11518,8 +12127,14 @@
         <f>VLOOKUP(C15,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>86.17</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -11534,8 +12149,14 @@
         <f>VLOOKUP(C16,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>94.91</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -11550,8 +12171,15 @@
         <f>VLOOKUP(C17,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>91.32</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="str">
+        <f>VLOOKUP(A17,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Syracuse</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
@@ -11565,8 +12193,15 @@
         <f>VLOOKUP(C18,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>70.040000000000006</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="e">
+        <f>VLOOKUP(A18,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -11581,8 +12216,15 @@
         <f>VLOOKUP(C19,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>78.599999999999994</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="e">
+        <f>VLOOKUP(A19,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -11596,8 +12238,15 @@
         <f>VLOOKUP(C20,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>80.930000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="e">
+        <f>VLOOKUP(A20,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -11612,8 +12261,14 @@
         <f>VLOOKUP(C21,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>80.89</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -11627,8 +12282,15 @@
         <f>VLOOKUP(C22,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>81.34</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="str">
+        <f>VLOOKUP(A22,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>VCU</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -11643,8 +12305,15 @@
         <f>VLOOKUP(C23,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>79.260000000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="e">
+        <f>VLOOKUP(A23,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -11658,8 +12327,15 @@
         <f>VLOOKUP(C24,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>81.13</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="e">
+        <f>VLOOKUP(A24,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -11673,8 +12349,15 @@
         <f>VLOOKUP(C25,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83.75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="e">
+        <f>VLOOKUP(A25,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -11689,8 +12372,14 @@
         <f>VLOOKUP(C26,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>84.35</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -11705,8 +12394,15 @@
         <f>VLOOKUP(C27,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>82.38</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="str">
+        <f>VLOOKUP(A27,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Notre Dame</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -11721,8 +12417,15 @@
         <f>VLOOKUP(C28,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.25</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="1" t="str">
+        <f>VLOOKUP(A28,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>UNLV</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -11737,8 +12440,15 @@
         <f>VLOOKUP(C29,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>89.47</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="e">
+        <f>VLOOKUP(A29,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -11753,8 +12463,15 @@
         <f>VLOOKUP(C30,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>89.55</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="1" t="str">
+        <f>VLOOKUP(A30,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Indiana</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -11769,8 +12486,15 @@
         <f>VLOOKUP(C31,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>87.99</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="1" t="e">
+        <f>VLOOKUP(A31,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -11785,8 +12509,15 @@
         <f>VLOOKUP(C32,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>88.27</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="1" t="str">
+        <f>VLOOKUP(A32,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Duke</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -11801,8 +12532,15 @@
         <f>VLOOKUP(C33,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>94.35</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="1" t="str">
+        <f>VLOOKUP(A33,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Kentucky</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -11817,8 +12555,15 @@
         <f>VLOOKUP(C34,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>74.84</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="1" t="e">
+        <f>VLOOKUP(A34,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -11833,8 +12578,15 @@
         <f>VLOOKUP(C35,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>75.84</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="1" t="e">
+        <f>VLOOKUP(A35,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -11849,8 +12601,15 @@
         <f>VLOOKUP(C36,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="1" t="e">
+        <f>VLOOKUP(A36,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -11865,8 +12624,15 @@
         <f>VLOOKUP(C37,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>79.86</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="1" t="str">
+        <f>VLOOKUP(A37,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Ohio</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>66</v>
       </c>
@@ -11881,8 +12647,15 @@
         <f>VLOOKUP(C38,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>79.94</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="1" t="e">
+        <f>VLOOKUP(A38,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -11897,8 +12670,15 @@
         <f>VLOOKUP(C39,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>82.63</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="1" t="e">
+        <f>VLOOKUP(A39,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -11913,8 +12693,15 @@
         <f>VLOOKUP(C40,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.14</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="1" t="e">
+        <f>VLOOKUP(A40,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -11929,8 +12716,15 @@
         <f>VLOOKUP(C41,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.26</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="1" t="str">
+        <f>VLOOKUP(A41,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Alabama</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -11945,8 +12739,15 @@
         <f>VLOOKUP(C42,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>84.77</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="1" t="e">
+        <f>VLOOKUP(A42,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -11960,8 +12761,15 @@
         <f>VLOOKUP(C43,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>62.93</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="1" t="e">
+        <f>VLOOKUP(A43,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -11975,8 +12783,15 @@
         <f>VLOOKUP(C44,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>81.39</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="1" t="str">
+        <f>VLOOKUP(A44,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>San Diego St.</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -11991,8 +12806,15 @@
         <f>VLOOKUP(C45,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83.52</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="1" t="str">
+        <f>VLOOKUP(A45,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Temple</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -12007,8 +12829,15 @@
         <f>VLOOKUP(C46,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.13</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="1" t="str">
+        <f>VLOOKUP(A46,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Michigan</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -12023,8 +12852,15 @@
         <f>VLOOKUP(C47,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>88.11</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="1" t="str">
+        <f>VLOOKUP(A47,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Georgetown</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -12039,8 +12875,15 @@
         <f>VLOOKUP(C48,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>92.45</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="1" t="str">
+        <f>VLOOKUP(A48,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Kansas</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -12055,8 +12898,15 @@
         <f>VLOOKUP(C49,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>91.85</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="1" t="str">
+        <f>VLOOKUP(A49,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>North Carolina</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -12070,8 +12920,15 @@
         <f>VLOOKUP(C50,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>72.75</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="1" t="e">
+        <f>VLOOKUP(A50,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -12086,8 +12943,15 @@
         <f>VLOOKUP(C51,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>70.52</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="1" t="e">
+        <f>VLOOKUP(A51,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
@@ -12102,8 +12966,15 @@
         <f>VLOOKUP(C52,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83.23</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="1" t="e">
+        <f>VLOOKUP(A52,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -12118,8 +12989,15 @@
         <f>VLOOKUP(C53,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>80.349999999999994</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="1" t="e">
+        <f>VLOOKUP(A53,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -12134,8 +13012,14 @@
         <f>VLOOKUP(C54,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>83</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -12150,8 +13034,14 @@
         <f>VLOOKUP(C55,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>79.31</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -12166,8 +13056,15 @@
         <f>VLOOKUP(C56,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>85.4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="1" t="str">
+        <f>VLOOKUP(A56,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Virginia</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -12182,8 +13079,15 @@
         <f>VLOOKUP(C57,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>87.33</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="1" t="str">
+        <f>VLOOKUP(A57,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Saint Louis</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -12198,8 +13102,15 @@
         <f>VLOOKUP(C58,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>88.74</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="1" t="str">
+        <f>VLOOKUP(A58,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Memphis</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -12214,8 +13125,15 @@
         <f>VLOOKUP(C59,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>87.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="1" t="str">
+        <f>VLOOKUP(A59,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Florida</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -12230,8 +13148,15 @@
         <f>VLOOKUP(C60,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>82.01</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="1" t="e">
+        <f>VLOOKUP(A60,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -12246,8 +13171,15 @@
         <f>VLOOKUP(C61,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>87.37</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="1" t="str">
+        <f>VLOOKUP(A61,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>New Mexico</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -12262,8 +13194,15 @@
         <f>VLOOKUP(C62,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>86.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="1" t="str">
+        <f>VLOOKUP(A62,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Louisville</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -12278,8 +13217,15 @@
         <f>VLOOKUP(C63,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>87.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="1" t="e">
+        <f>VLOOKUP(A63,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -12294,8 +13240,15 @@
         <f>VLOOKUP(C64,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>90.9</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="1" t="str">
+        <f>VLOOKUP(A64,usaTodayNames!$A$1:$A$80,1,)</f>
+        <v>Missouri</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -12309,6 +13262,12 @@
       <c r="D65">
         <f>VLOOKUP(C65,'2012.03.12 Sagarin Ratings'!$A$2:$D$346,4,FALSE)</f>
         <v>93.12</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>